<commit_message>
New Sourcemessages Template File
</commit_message>
<xml_diff>
--- a/modules/main/templates/sourcemessage_last.xlsx
+++ b/modules/main/templates/sourcemessage_last.xlsx
@@ -7,19 +7,19 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="TR_EXCEL_TITLE26-05-2016-15-03" sheetId="1" r:id="rId4"/>
+    <sheet name="TR_EXCEL_TITLE29-05-2016-14-24" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TR_EXCEL_TITLE26-05-2016-15-03'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TR_EXCEL_TITLE29-05-2016-14-24'!$A$3:$D$3</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="461">
-  <si>
-    <t>TRANSLATION_EXCEL_TABLEHEADER_26.05.2016 15:03</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="495">
+  <si>
+    <t>TRANSLATION_EXCEL_TABLEHEADER_29.05.2016 14:24</t>
   </si>
   <si>
     <t>Категория</t>
@@ -85,12 +85,6 @@
     <t>Поиск</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Сброс</t>
-  </si>
-  <si>
     <t>Source Messages</t>
   </si>
   <si>
@@ -211,7 +205,7 @@
     <t>{icon} RESTORE</t>
   </si>
   <si>
-    <t>{icon} Восстановить</t>
+    <t>{icon} Восст.</t>
   </si>
   <si>
     <t>ERROR_EMAIL_EXISTS</t>
@@ -859,135 +853,132 @@
     <t>{icon} ŠKODA. Монитор готовности</t>
   </si>
   <si>
-    <t>{icon} EXCEL_OPERATIONS</t>
+    <t>{icon} IMPORT_EXCEL</t>
+  </si>
+  <si>
+    <t>{icon} Импорт Excel</t>
+  </si>
+  <si>
+    <t>{icon} SERVICESHEDULER</t>
+  </si>
+  <si>
+    <t>{icon} График смен</t>
+  </si>
+  <si>
+    <t>{icon} STATUSMONITOR</t>
+  </si>
+  <si>
+    <t>{icon} Монитор готовности</t>
+  </si>
+  <si>
+    <t>CLIENTCIRCULATION</t>
+  </si>
+  <si>
+    <t>ОКиС. Трафик клиентов</t>
+  </si>
+  <si>
+    <t>{icon} ADD_EVENT</t>
+  </si>
+  <si>
+    <t>{icon} Добавить событие</t>
+  </si>
+  <si>
+    <t>{icon} CLIENTCIRCULATION</t>
+  </si>
+  <si>
+    <t>{icon} ОКиС. Трафик Клиентов</t>
+  </si>
+  <si>
+    <t>CLIENTNAME</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>Регион</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t>Сотрудники</t>
+  </si>
+  <si>
+    <t>CONTACT_TYPE</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>CAR_MODEL</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>WORKSHEDULER_DATE</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>WORKSHEDULER_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>Ответственный</t>
+  </si>
+  <si>
+    <t>MASTER_CONSULTANT_DOES_NOT_EXIST_TODAY</t>
+  </si>
+  <si>
+    <t>Не назначен мастер-консультант на текущую дату</t>
+  </si>
+  <si>
+    <t>CURRENT_MASTER_CONSULTANT</t>
+  </si>
+  <si>
+    <t>Мастер-консультант</t>
+  </si>
+  <si>
+    <t>SERVICESHEDULER_INDEX</t>
+  </si>
+  <si>
+    <t>График смен</t>
+  </si>
+  <si>
+    <t>SERVICESHEDULER_CALENDAR</t>
+  </si>
+  <si>
+    <t>Календарь</t>
+  </si>
+  <si>
+    <t>SERVICESHEDULER_TABLE</t>
+  </si>
+  <si>
+    <t>Таблица</t>
+  </si>
+  <si>
+    <t>{icon} STATUS_CREATE</t>
+  </si>
+  <si>
+    <t>{icon} STATUS_REFRESH</t>
+  </si>
+  <si>
+    <t>{icon} STATUS_EXPORT_EXCEL</t>
   </si>
   <si>
     <t>{icon} Excel</t>
   </si>
   <si>
-    <t>{icon} IMPORT_EXCEL</t>
-  </si>
-  <si>
-    <t>{icon} Импорт Excel</t>
-  </si>
-  <si>
-    <t>{icon} SERVICESHEDULER</t>
-  </si>
-  <si>
-    <t>{icon} График смен</t>
-  </si>
-  <si>
-    <t>{icon} STATUSMONITOR</t>
-  </si>
-  <si>
-    <t>{icon} Монитор готовности</t>
-  </si>
-  <si>
-    <t>CLIENTCIRCULATION</t>
-  </si>
-  <si>
-    <t>ОКиС. Трафик клиентов</t>
-  </si>
-  <si>
-    <t>{icon} ADD_EVENT</t>
-  </si>
-  <si>
-    <t>{icon} Добавить событие</t>
-  </si>
-  <si>
-    <t>{icon} CLIENTCIRCULATION</t>
-  </si>
-  <si>
-    <t>{icon} ОКиС. Трафик Клиентов</t>
-  </si>
-  <si>
-    <t>CLIENTNAME</t>
-  </si>
-  <si>
-    <t>PHONE</t>
-  </si>
-  <si>
-    <t>Телефон</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>REGION</t>
-  </si>
-  <si>
-    <t>Регион</t>
-  </si>
-  <si>
-    <t>EMPLOYEE</t>
-  </si>
-  <si>
-    <t>Сотрудники</t>
-  </si>
-  <si>
-    <t>CONTACT_TYPE</t>
-  </si>
-  <si>
-    <t>TARGET</t>
-  </si>
-  <si>
-    <t>CAR_MODEL</t>
-  </si>
-  <si>
-    <t>COMMENT</t>
-  </si>
-  <si>
-    <t>WORKSHEDULER_DATE</t>
-  </si>
-  <si>
-    <t>Дата</t>
-  </si>
-  <si>
-    <t>WORKSHEDULER_RESPONSIBLE</t>
-  </si>
-  <si>
-    <t>Ответственный</t>
-  </si>
-  <si>
-    <t>MASTER_CONSULTANT_DOES_NOT_EXIST_TODAY</t>
-  </si>
-  <si>
-    <t>Не назначен мастер-консультант на текущую дату</t>
-  </si>
-  <si>
-    <t>CURRENT_MASTER_CONSULTANT</t>
-  </si>
-  <si>
-    <t>Мастер-консультант</t>
-  </si>
-  <si>
-    <t>SERVICESHEDULER_INDEX</t>
-  </si>
-  <si>
-    <t>График смен</t>
-  </si>
-  <si>
-    <t>SERVICESHEDULER_CALENDAR</t>
-  </si>
-  <si>
-    <t>Календарь</t>
-  </si>
-  <si>
-    <t>SERVICESHEDULER_TABLE</t>
-  </si>
-  <si>
-    <t>Таблица</t>
-  </si>
-  <si>
-    <t>{icon} STATUS_CREATE</t>
-  </si>
-  <si>
-    <t>{icon} STATUS_REFRESH</t>
-  </si>
-  <si>
-    <t>{icon} STATUS_EXPORT_EXCEL</t>
-  </si>
-  <si>
     <t>SERVICESHEDULER_CREATE</t>
   </si>
   <si>
@@ -1081,9 +1072,15 @@
     <t>ERROR_WORKSHEDULER_DOES_NOT_EXIST_TO</t>
   </si>
   <si>
+    <t>Не назначен мастер-консультант на дату выдачи а/м</t>
+  </si>
+  <si>
     <t>ERROR_WORKSHEDULER_DOES_NOT_EXIST_FROM</t>
   </si>
   <si>
+    <t>Не назначен мастер-консультант на дату приема а/м</t>
+  </si>
+  <si>
     <t>{icon} STATUSMONITOR_TABLE</t>
   </si>
   <si>
@@ -1282,6 +1279,9 @@
     <t>IMPORTEXCEL</t>
   </si>
   <si>
+    <t>Импорт</t>
+  </si>
+  <si>
     <t>ADMIN_POSITIONS_POSITION</t>
   </si>
   <si>
@@ -1400,6 +1400,108 @@
   </si>
   <si>
     <t>Выгрузить отмеченные записи в Excel?</t>
+  </si>
+  <si>
+    <t>{icon} SERVICESHEDULER_GRAPH</t>
+  </si>
+  <si>
+    <t>{icon} График</t>
+  </si>
+  <si>
+    <t>{icon} SERVICESHEDULER_INDEX</t>
+  </si>
+  <si>
+    <t>{icon} ADVANCED</t>
+  </si>
+  <si>
+    <t>{icon} Дополнительно</t>
+  </si>
+  <si>
+    <t>CREDITCALENDARS</t>
+  </si>
+  <si>
+    <t>ОКиС. Календарь</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_EXPORT_EXCEL</t>
+  </si>
+  <si>
+    <t>RESPONSIBLES_DOES_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>Ответственные не назначены</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>Комментарии</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_CALENDAR</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_TABLE</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_TABLE_ALL</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_TABLE_PRIVATE</t>
+  </si>
+  <si>
+    <t>{icon} Таблица (личные)</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_GRAPH</t>
+  </si>
+  <si>
+    <t>CREDITCALENDAR</t>
+  </si>
+  <si>
+    <t>Календарь.</t>
+  </si>
+  <si>
+    <t>{icon} CHECK_ALL</t>
+  </si>
+  <si>
+    <t>{icon} Отметить все</t>
+  </si>
+  <si>
+    <t>{icon} UNCHECK_ALL</t>
+  </si>
+  <si>
+    <t>{icon} Снять отметки</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_PRIVATE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>{icon} Личная запись</t>
+  </si>
+  <si>
+    <t>{icon} CREDITCALENDAR_ALLDAY_CHECKBOX</t>
+  </si>
+  <si>
+    <t>{icon} Ежедневно</t>
+  </si>
+  <si>
+    <t>{icon} COMMENTS</t>
+  </si>
+  <si>
+    <t>{icon} Комментарии</t>
+  </si>
+  <si>
+    <t>{icon} COMMENT</t>
+  </si>
+  <si>
+    <t>{icon} Комментарий</t>
+  </si>
+  <si>
+    <t>YOU_CANNOT_EXECUTE_THIS_ACTION</t>
+  </si>
+  <si>
+    <t>Вам запрещено выполнять данное действие</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1905,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D295"/>
+  <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2017,16 +2119,14 @@
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
@@ -2038,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
@@ -2050,12 +2150,14 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
@@ -2165,34 +2267,34 @@
       <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2200,13 +2302,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2234,7 +2336,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2242,13 +2344,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2317,21 +2419,21 @@
       <c r="C38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
@@ -2358,7 +2460,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2366,13 +2468,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2386,7 +2488,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2394,13 +2496,13 @@
         <v>5</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2428,7 +2530,7 @@
         <v>7</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2436,13 +2538,13 @@
         <v>5</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2456,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2464,13 +2566,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2484,7 +2586,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2492,13 +2594,13 @@
         <v>5</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2637,16 +2739,14 @@
       <c r="C61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>7</v>
@@ -2658,12 +2758,14 @@
         <v>5</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
@@ -2871,16 +2973,14 @@
       <c r="C78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>7</v>
@@ -2892,7 +2992,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>7</v>
@@ -2904,25 +3004,27 @@
         <v>5</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2978,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2986,13 +3088,13 @@
         <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3006,7 +3108,7 @@
         <v>7</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>151</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3014,7 +3116,7 @@
         <v>5</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>7</v>
@@ -3028,7 +3130,7 @@
         <v>5</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>7</v>
@@ -3042,13 +3144,13 @@
         <v>5</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3061,16 +3163,14 @@
       <c r="C92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>7</v>
@@ -3082,12 +3182,14 @@
         <v>5</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
@@ -3128,7 +3230,7 @@
         <v>7</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>164</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3136,26 +3238,26 @@
         <v>5</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
@@ -3182,7 +3284,7 @@
         <v>7</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3190,13 +3292,13 @@
         <v>5</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3204,13 +3306,13 @@
         <v>5</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3218,13 +3320,13 @@
         <v>5</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3252,7 +3354,7 @@
         <v>7</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3260,13 +3362,13 @@
         <v>5</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3294,7 +3396,7 @@
         <v>7</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3302,26 +3404,26 @@
         <v>5</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="D110" s="2"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D111" s="2"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
@@ -3334,7 +3436,7 @@
         <v>7</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>186</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3342,13 +3444,13 @@
         <v>5</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3356,13 +3458,13 @@
         <v>5</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3390,7 +3492,7 @@
         <v>7</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>192</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3398,39 +3500,39 @@
         <v>5</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D117" s="2"/>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D118" s="2"/>
+      <c r="D118" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3438,7 +3540,7 @@
         <v>5</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>7</v>
@@ -3452,21 +3554,19 @@
         <v>5</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>7</v>
@@ -3478,7 +3578,7 @@
         <v>5</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>7</v>
@@ -3490,12 +3590,14 @@
         <v>5</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D124" s="2"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
@@ -3522,7 +3624,7 @@
         <v>7</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3530,7 +3632,7 @@
         <v>5</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>7</v>
@@ -3544,13 +3646,13 @@
         <v>5</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3563,16 +3665,14 @@
       <c r="C129" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>208</v>
-      </c>
+      <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>7</v>
@@ -3584,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>7</v>
@@ -3596,7 +3696,7 @@
         <v>5</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>7</v>
@@ -3608,25 +3708,27 @@
         <v>5</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="2"/>
+      <c r="D133" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3639,21 +3741,21 @@
       <c r="C135" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>215</v>
-      </c>
+      <c r="D135" s="2"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D136" s="2"/>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
@@ -3666,7 +3768,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3674,13 +3776,13 @@
         <v>5</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3694,7 +3796,7 @@
         <v>7</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>221</v>
+        <v>144</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3702,26 +3804,26 @@
         <v>5</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="D140" s="2"/>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B141" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D141" s="2"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2" t="s">
@@ -3832,7 +3934,7 @@
         <v>7</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>239</v>
+        <v>84</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3840,13 +3942,13 @@
         <v>5</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3888,7 +3990,7 @@
         <v>7</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3896,13 +3998,13 @@
         <v>5</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3910,13 +4012,13 @@
         <v>5</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3958,7 +4060,7 @@
         <v>7</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3966,13 +4068,13 @@
         <v>5</v>
       </c>
       <c r="B159" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4000,7 +4102,7 @@
         <v>7</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>259</v>
+        <v>102</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4008,13 +4110,13 @@
         <v>5</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4084,7 +4186,7 @@
         <v>7</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>270</v>
+        <v>78</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4092,13 +4194,13 @@
         <v>5</v>
       </c>
       <c r="B168" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4162,27 +4264,25 @@
         <v>5</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>280</v>
+        <v>67</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D173" s="2" t="s">
-        <v>281</v>
-      </c>
+      <c r="D173" s="2"/>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4190,12 +4290,14 @@
         <v>5</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>69</v>
+        <v>282</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D175" s="2"/>
+      <c r="D175" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="2" t="s">
@@ -4250,7 +4352,7 @@
         <v>7</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>291</v>
+        <v>86</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4258,13 +4360,13 @@
         <v>5</v>
       </c>
       <c r="B180" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4272,7 +4374,7 @@
         <v>5</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>294</v>
+        <v>88</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>7</v>
@@ -4286,13 +4388,13 @@
         <v>5</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>296</v>
+        <v>38</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4300,13 +4402,13 @@
         <v>5</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>90</v>
+        <v>294</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>90</v>
+        <v>295</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4314,13 +4416,13 @@
         <v>5</v>
       </c>
       <c r="B184" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D184" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4334,7 +4436,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>299</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4342,13 +4444,13 @@
         <v>5</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>301</v>
+        <v>32</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4356,13 +4458,13 @@
         <v>5</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4370,13 +4472,13 @@
         <v>5</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4384,13 +4486,13 @@
         <v>5</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>36</v>
+        <v>303</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4398,13 +4500,13 @@
         <v>5</v>
       </c>
       <c r="B190" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4488,7 +4590,7 @@
         <v>7</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>317</v>
+        <v>56</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4496,13 +4598,13 @@
         <v>5</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>319</v>
+        <v>58</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4510,13 +4612,13 @@
         <v>5</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>58</v>
+        <v>319</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4524,13 +4626,13 @@
         <v>5</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4538,13 +4640,13 @@
         <v>5</v>
       </c>
       <c r="B200" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4558,7 +4660,7 @@
         <v>7</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4572,7 +4674,7 @@
         <v>7</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>325</v>
+        <v>84</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4580,13 +4682,13 @@
         <v>5</v>
       </c>
       <c r="B203" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4600,7 +4702,7 @@
         <v>7</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4628,7 +4730,7 @@
         <v>7</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>25</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4636,13 +4738,13 @@
         <v>5</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>332</v>
+        <v>180</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4670,7 +4772,7 @@
         <v>7</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>182</v>
+        <v>336</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4678,13 +4780,13 @@
         <v>5</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4692,13 +4794,13 @@
         <v>5</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4726,7 +4828,7 @@
         <v>7</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4734,13 +4836,13 @@
         <v>5</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4748,13 +4850,13 @@
         <v>5</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>346</v>
+        <v>305</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4768,7 +4870,7 @@
         <v>7</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>348</v>
+        <v>38</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4776,13 +4878,13 @@
         <v>5</v>
       </c>
       <c r="B217" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D217" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4796,7 +4898,7 @@
         <v>7</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>40</v>
+        <v>351</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4804,13 +4906,13 @@
         <v>5</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4818,37 +4920,41 @@
         <v>5</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D220" s="2"/>
+      <c r="D220" s="2" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D221" s="2"/>
+      <c r="D221" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>356</v>
+        <v>19</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -4856,13 +4962,13 @@
         <v>5</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>358</v>
+        <v>19</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -4870,13 +4976,13 @@
         <v>5</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -4884,13 +4990,13 @@
         <v>5</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>19</v>
+        <v>362</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -4898,13 +5004,13 @@
         <v>5</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>15</v>
+        <v>364</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -4912,13 +5018,13 @@
         <v>5</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -4926,13 +5032,13 @@
         <v>5</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -4940,13 +5046,13 @@
         <v>5</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -4954,13 +5060,13 @@
         <v>5</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -4968,27 +5074,25 @@
         <v>5</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D231" s="2" t="s">
-        <v>371</v>
-      </c>
+      <c r="D231" s="2"/>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -4996,25 +5100,27 @@
         <v>5</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D233" s="2"/>
+      <c r="D233" s="2" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5022,13 +5128,13 @@
         <v>5</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>378</v>
+        <v>216</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5036,13 +5142,13 @@
         <v>5</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5050,13 +5156,13 @@
         <v>5</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>218</v>
+        <v>372</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5064,13 +5170,13 @@
         <v>5</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5078,13 +5184,13 @@
         <v>5</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>373</v>
+        <v>160</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5092,13 +5198,13 @@
         <v>5</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>369</v>
+        <v>158</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5106,7 +5212,7 @@
         <v>5</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>7</v>
@@ -5120,13 +5226,13 @@
         <v>5</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>160</v>
+        <v>388</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5134,13 +5240,13 @@
         <v>5</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>164</v>
+        <v>390</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5148,13 +5254,13 @@
         <v>5</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>389</v>
+        <v>166</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5162,13 +5268,13 @@
         <v>5</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5176,13 +5282,13 @@
         <v>5</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>168</v>
+        <v>370</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5190,13 +5296,13 @@
         <v>5</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5204,13 +5310,13 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>371</v>
+        <v>398</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5218,13 +5324,13 @@
         <v>5</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5232,13 +5338,13 @@
         <v>5</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5246,13 +5352,13 @@
         <v>5</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>401</v>
+        <v>295</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5260,13 +5366,13 @@
         <v>5</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>369</v>
+        <v>404</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5274,13 +5380,13 @@
         <v>5</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5288,13 +5394,13 @@
         <v>5</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>405</v>
+        <v>297</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5302,27 +5408,25 @@
         <v>5</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>299</v>
-      </c>
+      <c r="D255" s="2"/>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>301</v>
+        <v>409</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5330,25 +5434,27 @@
         <v>5</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D257" s="2"/>
+      <c r="D257" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5356,7 +5462,7 @@
         <v>5</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>7</v>
@@ -5370,13 +5476,13 @@
         <v>5</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5384,7 +5490,7 @@
         <v>5</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>7</v>
@@ -5398,13 +5504,13 @@
         <v>5</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5412,13 +5518,13 @@
         <v>5</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>114</v>
+        <v>420</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5426,21 +5532,19 @@
         <v>5</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D264" s="2" t="s">
-        <v>419</v>
-      </c>
+      <c r="D264" s="2"/>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>7</v>
@@ -5452,7 +5556,7 @@
         <v>5</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>7</v>
@@ -5464,37 +5568,41 @@
         <v>5</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D267" s="2"/>
+      <c r="D267" s="2" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D268" s="2"/>
+      <c r="D268" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5502,13 +5610,13 @@
         <v>5</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5516,13 +5624,13 @@
         <v>5</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5530,13 +5638,13 @@
         <v>5</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>116</v>
+        <v>433</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5544,13 +5652,13 @@
         <v>5</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5558,13 +5666,13 @@
         <v>5</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>433</v>
+        <v>180</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5572,13 +5680,13 @@
         <v>5</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>435</v>
+        <v>379</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5586,13 +5694,13 @@
         <v>5</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5600,27 +5708,25 @@
         <v>5</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D277" s="2" t="s">
-        <v>380</v>
-      </c>
+      <c r="D277" s="2"/>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>126</v>
+        <v>441</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5628,25 +5734,27 @@
         <v>5</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D279" s="2"/>
+      <c r="D279" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>441</v>
+        <v>116</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5654,13 +5762,13 @@
         <v>5</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>124</v>
+        <v>400</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5668,13 +5776,13 @@
         <v>5</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5682,13 +5790,13 @@
         <v>5</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>401</v>
+        <v>447</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5696,13 +5804,13 @@
         <v>5</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>122</v>
+        <v>449</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5710,13 +5818,13 @@
         <v>5</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5724,13 +5832,13 @@
         <v>5</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>449</v>
+        <v>126</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5738,13 +5846,13 @@
         <v>5</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>451</v>
+        <v>412</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5752,13 +5860,13 @@
         <v>5</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>128</v>
+        <v>412</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5766,35 +5874,31 @@
         <v>5</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D289" s="2" t="s">
-        <v>413</v>
-      </c>
+      <c r="D289" s="2"/>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D290" s="2" t="s">
-        <v>413</v>
-      </c>
+      <c r="D290" s="2"/>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>7</v>
@@ -5806,7 +5910,7 @@
         <v>5</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>7</v>
@@ -5818,37 +5922,291 @@
         <v>5</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D293" s="2"/>
+      <c r="D293" s="2" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D294" s="2"/>
+      <c r="D294" s="2" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>460</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D296" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
+      <c r="A298" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D298" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="A300" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
+      <c r="A302" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D303" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
+      <c r="A304" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="A305" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D305" s="2"/>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D306" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="A307" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D307" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4">
+      <c r="A308" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D309" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="A310" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D310" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
+      <c r="A311" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="A312" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
+      <c r="A313" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D313" s="2" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>